<commit_message>
Extract printed page setup from xlsx reader into its own class
</commit_message>
<xml_diff>
--- a/tests/data/Reader/XLSX/stylesTest.xlsx
+++ b/tests/data/Reader/XLSX/stylesTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PHPSpreadsheet\develop\tests\data\Reader\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{552A2A88-210A-430D-B6FB-684D0B3F9C75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302D87FA-8478-46C2-95D2-8D9493B188B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5123" yWindow="765" windowWidth="22830" windowHeight="13237" xr2:uid="{77B54B54-3A9D-489C-AF8D-F8B860992834}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -108,13 +108,19 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>HELLO WORLD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +187,54 @@
     <font>
       <sz val="11"/>
       <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -254,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -262,11 +316,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="1">
+      <left style="thick">
+        <color theme="9"/>
+      </left>
+      <right style="thick">
+        <color theme="4"/>
+      </right>
+      <top style="thick">
+        <color theme="5"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="medium">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1">
+      <left style="thick">
+        <color theme="4"/>
+      </left>
+      <right style="thick">
+        <color theme="9"/>
+      </right>
+      <top style="thick">
+        <color theme="5"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="medium">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="9"/>
+      </left>
+      <right style="thick">
+        <color theme="4"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="4"/>
+      </left>
+      <right style="thick">
+        <color theme="9"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -304,30 +422,63 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,29 +793,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4610FEFA-F717-4B69-B082-BF89EEEF9AC5}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="22" t="s">
         <v>9</v>
       </c>
     </row>
@@ -695,10 +848,10 @@
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="23">
         <v>1</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="25">
         <v>2</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -715,10 +868,10 @@
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <v>3</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="14">
         <v>4</v>
       </c>
       <c r="E4" s="9" t="s">
@@ -735,10 +888,10 @@
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="24">
         <v>5</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="26">
         <v>6</v>
       </c>
       <c r="E5" s="10" t="s">
@@ -755,10 +908,10 @@
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="15">
         <v>7</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="16">
         <v>8</v>
       </c>
       <c r="E6" s="10" t="s">
@@ -808,7 +961,39 @@
         <v>23</v>
       </c>
     </row>
+    <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="D10" s="30">
+        <v>1234.56</v>
+      </c>
+      <c r="F10" s="31"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+    </row>
+    <row r="12" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>